<commit_message>
Endpoint de sectores  y excel
</commit_message>
<xml_diff>
--- a/swagger_server/template_report.xlsx
+++ b/swagger_server/template_report.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -38,8 +38,17 @@
       <sz val="10"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -50,6 +59,18 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -114,18 +135,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -160,14 +175,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -175,10 +182,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
@@ -187,11 +190,58 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -611,170 +661,194 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
     <col width="3.28515625" customWidth="1" min="1" max="1"/>
     <col width="32.85546875" customWidth="1" min="2" max="2"/>
-    <col width="18" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="16.140625" customWidth="1" min="3" max="3"/>
     <col width="10" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="6.28515625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="10.85546875" customWidth="1" min="5" max="5"/>
     <col width="11.140625" bestFit="1" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="n"/>
-      <c r="B1" s="6" t="n"/>
-      <c r="C1" s="6" t="n"/>
-      <c r="D1" s="6" t="n"/>
-      <c r="E1" s="6" t="n"/>
-      <c r="F1" s="6" t="n"/>
+      <c r="A1" s="4" t="n"/>
+      <c r="B1" s="4" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="4" t="n"/>
+      <c r="E1" s="4" t="n"/>
+      <c r="F1" s="4" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="n"/>
-      <c r="B2" s="6" t="n"/>
-      <c r="C2" s="6" t="n"/>
-      <c r="D2" s="6" t="n"/>
-      <c r="E2" s="6" t="n"/>
-      <c r="F2" s="6" t="n"/>
+      <c r="A2" s="4" t="n"/>
+      <c r="B2" s="4" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="4" t="n"/>
+      <c r="E2" s="4" t="n"/>
+      <c r="F2" s="4" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="n"/>
-      <c r="B3" s="6" t="n"/>
-      <c r="C3" s="6" t="n"/>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="6" t="n"/>
-      <c r="F3" s="6" t="n"/>
+      <c r="A3" s="4" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="4" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="4" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="n"/>
-      <c r="B4" s="6" t="n"/>
-      <c r="C4" s="6" t="n"/>
-      <c r="D4" s="6" t="n"/>
-      <c r="E4" s="6" t="n"/>
-      <c r="F4" s="6" t="n"/>
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="4" t="n"/>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="4" t="n"/>
+      <c r="E4" s="4" t="n"/>
+      <c r="F4" s="4" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="n"/>
-      <c r="B5" s="6" t="n"/>
-      <c r="C5" s="6" t="n"/>
-      <c r="D5" s="6" t="n"/>
-      <c r="E5" s="6" t="n"/>
-      <c r="F5" s="6" t="n"/>
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="4" t="n"/>
+      <c r="E5" s="4" t="n"/>
+      <c r="F5" s="4" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="n"/>
-      <c r="B6" s="6" t="n"/>
-      <c r="C6" s="6" t="n"/>
-      <c r="D6" s="6" t="n"/>
-      <c r="E6" s="6" t="n"/>
-      <c r="F6" s="6" t="n"/>
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="4" t="n"/>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="4" t="n"/>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="n"/>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">FECHA </t>
         </is>
       </c>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="8" t="n"/>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="C7" s="17" t="inlineStr">
+        <is>
+          <t>28/01/2026</t>
+        </is>
+      </c>
+      <c r="D7" s="27" t="n"/>
+      <c r="E7" s="7" t="inlineStr">
         <is>
           <t>REP#</t>
         </is>
       </c>
-      <c r="F7" s="5" t="n"/>
+      <c r="F7" s="18" t="inlineStr">
+        <is>
+          <t>RP2026-010</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="n"/>
-      <c r="B8" s="7" t="inlineStr">
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>LOCALIDAD</t>
         </is>
       </c>
-      <c r="C8" s="5" t="n"/>
-      <c r="D8" s="8" t="n"/>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="C8" s="18" t="inlineStr">
+        <is>
+          <t>TAURA (TOTAL)</t>
+        </is>
+      </c>
+      <c r="D8" s="27" t="n"/>
+      <c r="E8" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">HORA </t>
         </is>
       </c>
-      <c r="F8" s="5" t="n"/>
+      <c r="F8" s="20" t="inlineStr">
+        <is>
+          <t>16:01:17</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>PUESTO DE CONTROL</t>
         </is>
       </c>
-      <c r="C9" s="18" t="n"/>
-      <c r="D9" s="21" t="n"/>
-      <c r="E9" s="8" t="n"/>
-      <c r="F9" s="8" t="n"/>
+      <c r="C9" s="19" t="inlineStr">
+        <is>
+          <t>GARITA DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="D9" s="27" t="n"/>
+      <c r="E9" s="7" t="n"/>
+      <c r="F9" s="3" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="n"/>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>AGENTE SEGURIDAD</t>
         </is>
       </c>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="8" t="n"/>
-      <c r="E10" s="8" t="n"/>
-      <c r="F10" s="8" t="n"/>
+      <c r="C10" s="16" t="inlineStr">
+        <is>
+          <t>Juan Perez</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="n"/>
+      <c r="E10" s="6" t="n"/>
+      <c r="F10" s="6" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="n"/>
-      <c r="B11" s="11" t="n"/>
-      <c r="C11" s="10" t="n"/>
-      <c r="D11" s="8" t="n"/>
-      <c r="E11" s="8" t="n"/>
-      <c r="F11" s="8" t="n"/>
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="9" t="n"/>
+      <c r="C11" s="8" t="n"/>
+      <c r="D11" s="6" t="n"/>
+      <c r="E11" s="6" t="n"/>
+      <c r="F11" s="6" t="n"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="6" t="n"/>
-      <c r="B12" s="11" t="n"/>
-      <c r="C12" s="19" t="inlineStr">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="9" t="n"/>
+      <c r="C12" s="14" t="inlineStr">
         <is>
           <t>SALIDA</t>
         </is>
       </c>
-      <c r="D12" s="22" t="n"/>
-      <c r="E12" s="19" t="inlineStr">
+      <c r="D12" s="28" t="n"/>
+      <c r="E12" s="14" t="inlineStr">
         <is>
           <t>ENTRADA</t>
         </is>
       </c>
-      <c r="F12" s="22" t="n"/>
+      <c r="F12" s="28" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="12" t="inlineStr">
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">DESCRIPCIÓN </t>
         </is>
       </c>
-      <c r="C13" s="3" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">CANT </t>
         </is>
       </c>
-      <c r="D13" s="3" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>UNIDAD</t>
         </is>
       </c>
-      <c r="E13" s="3" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">CANT </t>
         </is>
       </c>
-      <c r="F13" s="3" t="inlineStr">
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>UNIDAD</t>
         </is>
@@ -782,545 +856,556 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
+      <c r="B14" s="29" t="inlineStr">
+        <is>
+          <t>TAURA (TOTAL)</t>
+        </is>
+      </c>
+      <c r="C14" s="22" t="n"/>
+      <c r="D14" s="22" t="n"/>
+      <c r="E14" s="22" t="n"/>
+      <c r="F14" s="22" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="18" t="inlineStr">
-        <is>
-          <t>TOTAL Camarón</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="D15" s="4" t="inlineStr">
-        <is>
-          <t>LIBRAS</t>
-        </is>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4" t="inlineStr">
-        <is>
-          <t>LIBRAS</t>
-        </is>
-      </c>
+      <c r="B15" s="30" t="inlineStr">
+        <is>
+          <t>CAMANGLAR 1</t>
+        </is>
+      </c>
+      <c r="C15" s="23" t="n"/>
+      <c r="D15" s="24" t="n"/>
+      <c r="E15" s="23" t="n"/>
+      <c r="F15" s="24" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="16" t="inlineStr">
-        <is>
-          <t>TOTAL Tilapia</t>
-        </is>
-      </c>
-      <c r="C16" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D16" s="4" t="inlineStr">
-        <is>
-          <t>LIBRAS</t>
-        </is>
-      </c>
-      <c r="E16" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F16" s="4" t="inlineStr">
-        <is>
-          <t>LIBRAS</t>
+      <c r="B16" s="12" t="inlineStr">
+        <is>
+          <t>TOTAL TILAPIA</t>
+        </is>
+      </c>
+      <c r="C16" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="24" t="inlineStr">
+        <is>
+          <t>KILOGRAMO</t>
+        </is>
+      </c>
+      <c r="E16" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="24" t="inlineStr">
+        <is>
+          <t>KILOGRAMO</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="2" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="4" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="4" t="n"/>
+      <c r="B17" s="12" t="n"/>
+      <c r="C17" s="23" t="n"/>
+      <c r="D17" s="24" t="n"/>
+      <c r="E17" s="23" t="n"/>
+      <c r="F17" s="24" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="2" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="4" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="4" t="n"/>
+      <c r="B18" s="31" t="inlineStr">
+        <is>
+          <t>CAMANGLAR 2</t>
+        </is>
+      </c>
+      <c r="C18" s="23" t="n"/>
+      <c r="D18" s="24" t="n"/>
+      <c r="E18" s="23" t="n"/>
+      <c r="F18" s="24" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="2" t="n"/>
-      <c r="C19" s="5" t="n"/>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="5" t="n"/>
-      <c r="F19" s="4" t="n"/>
+      <c r="B19" s="12" t="inlineStr">
+        <is>
+          <t>TOTAL TILAPIA</t>
+        </is>
+      </c>
+      <c r="C19" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="24" t="inlineStr">
+        <is>
+          <t>KILOGRAMO</t>
+        </is>
+      </c>
+      <c r="E19" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="24" t="inlineStr">
+        <is>
+          <t>KILOGRAMO</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="2" t="n"/>
-      <c r="C20" s="5" t="n"/>
-      <c r="D20" s="4" t="n"/>
-      <c r="E20" s="5" t="n"/>
-      <c r="F20" s="4" t="n"/>
+      <c r="B20" s="12" t="n"/>
+      <c r="C20" s="23" t="n"/>
+      <c r="D20" s="24" t="n"/>
+      <c r="E20" s="23" t="n"/>
+      <c r="F20" s="24" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="2" t="n"/>
-      <c r="C21" s="5" t="n"/>
-      <c r="D21" s="4" t="n"/>
-      <c r="E21" s="5" t="n"/>
-      <c r="F21" s="4" t="n"/>
+      <c r="B21" s="12" t="n"/>
+      <c r="C21" s="23" t="n"/>
+      <c r="D21" s="24" t="n"/>
+      <c r="E21" s="23" t="n"/>
+      <c r="F21" s="24" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="2" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="4" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="4" t="n"/>
+      <c r="B22" s="12" t="n"/>
+      <c r="C22" s="23" t="n"/>
+      <c r="D22" s="24" t="n"/>
+      <c r="E22" s="23" t="n"/>
+      <c r="F22" s="24" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="2" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="4" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="4" t="n"/>
+      <c r="B23" s="12" t="n"/>
+      <c r="C23" s="23" t="n"/>
+      <c r="D23" s="24" t="n"/>
+      <c r="E23" s="23" t="n"/>
+      <c r="F23" s="24" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="2" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="4" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="4" t="n"/>
+      <c r="B24" s="12" t="n"/>
+      <c r="C24" s="23" t="n"/>
+      <c r="D24" s="24" t="n"/>
+      <c r="E24" s="23" t="n"/>
+      <c r="F24" s="24" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="2" t="n"/>
-      <c r="C25" s="5" t="n"/>
-      <c r="D25" s="4" t="n"/>
-      <c r="E25" s="5" t="n"/>
-      <c r="F25" s="4" t="n"/>
+      <c r="B25" s="12" t="n"/>
+      <c r="C25" s="23" t="n"/>
+      <c r="D25" s="24" t="n"/>
+      <c r="E25" s="23" t="n"/>
+      <c r="F25" s="24" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="2" t="n"/>
-      <c r="C26" s="5" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="5" t="n"/>
-      <c r="F26" s="4" t="n"/>
+      <c r="B26" s="12" t="n"/>
+      <c r="C26" s="23" t="n"/>
+      <c r="D26" s="24" t="n"/>
+      <c r="E26" s="23" t="n"/>
+      <c r="F26" s="24" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="2" t="n"/>
-      <c r="C27" s="5" t="n"/>
-      <c r="D27" s="4" t="n"/>
-      <c r="E27" s="5" t="n"/>
-      <c r="F27" s="4" t="n"/>
+      <c r="B27" s="12" t="n"/>
+      <c r="C27" s="23" t="n"/>
+      <c r="D27" s="24" t="n"/>
+      <c r="E27" s="23" t="n"/>
+      <c r="F27" s="24" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="2" t="n"/>
-      <c r="C28" s="5" t="n"/>
-      <c r="D28" s="4" t="n"/>
-      <c r="E28" s="5" t="n"/>
-      <c r="F28" s="4" t="n"/>
+      <c r="B28" s="12" t="n"/>
+      <c r="C28" s="23" t="n"/>
+      <c r="D28" s="24" t="n"/>
+      <c r="E28" s="23" t="n"/>
+      <c r="F28" s="24" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="n"/>
-      <c r="B29" s="15" t="n"/>
-      <c r="C29" s="15" t="n"/>
-      <c r="D29" s="15" t="n"/>
-      <c r="E29" s="15" t="n"/>
-      <c r="F29" s="15" t="n"/>
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" s="13" t="n"/>
+      <c r="C29" s="25" t="n"/>
+      <c r="D29" s="25" t="n"/>
+      <c r="E29" s="25" t="n"/>
+      <c r="F29" s="25" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="n"/>
-      <c r="B30" s="13" t="n"/>
-      <c r="C30" s="14" t="n"/>
-      <c r="D30" s="14" t="n"/>
-      <c r="E30" s="14" t="n"/>
-      <c r="F30" s="14" t="n"/>
+      <c r="A30" s="4" t="n"/>
+      <c r="B30" s="11" t="n"/>
+      <c r="C30" s="26" t="n"/>
+      <c r="D30" s="26" t="n"/>
+      <c r="E30" s="26" t="n"/>
+      <c r="F30" s="26" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="n"/>
-      <c r="B31" s="18" t="n"/>
-      <c r="C31" s="14" t="n"/>
-      <c r="D31" s="4" t="n"/>
-      <c r="E31" s="14" t="n"/>
-      <c r="F31" s="4" t="n"/>
+      <c r="A31" s="4" t="n"/>
+      <c r="B31" s="13" t="n"/>
+      <c r="C31" s="26" t="n"/>
+      <c r="D31" s="24" t="n"/>
+      <c r="E31" s="26" t="n"/>
+      <c r="F31" s="24" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="n"/>
-      <c r="B32" s="18" t="n"/>
-      <c r="C32" s="14" t="n"/>
-      <c r="D32" s="4" t="n"/>
-      <c r="E32" s="14" t="n"/>
-      <c r="F32" s="4" t="n"/>
+      <c r="A32" s="4" t="n"/>
+      <c r="B32" s="13" t="n"/>
+      <c r="C32" s="26" t="n"/>
+      <c r="D32" s="24" t="n"/>
+      <c r="E32" s="26" t="n"/>
+      <c r="F32" s="24" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="n"/>
-      <c r="B33" s="11" t="n"/>
-      <c r="C33" s="14" t="n"/>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="14" t="n"/>
-      <c r="F33" s="4" t="n"/>
+      <c r="A33" s="4" t="n"/>
+      <c r="B33" s="13" t="n"/>
+      <c r="C33" s="26" t="n"/>
+      <c r="D33" s="24" t="n"/>
+      <c r="E33" s="26" t="n"/>
+      <c r="F33" s="24" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="n"/>
-      <c r="B34" s="11" t="n"/>
-      <c r="C34" s="14" t="n"/>
-      <c r="D34" s="4" t="n"/>
-      <c r="E34" s="14" t="n"/>
-      <c r="F34" s="4" t="n"/>
+      <c r="A34" s="4" t="n"/>
+      <c r="B34" s="13" t="n"/>
+      <c r="C34" s="26" t="n"/>
+      <c r="D34" s="24" t="n"/>
+      <c r="E34" s="26" t="n"/>
+      <c r="F34" s="24" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="n"/>
-      <c r="B35" s="11" t="n"/>
-      <c r="C35" s="14" t="n"/>
-      <c r="D35" s="4" t="n"/>
-      <c r="E35" s="14" t="n"/>
-      <c r="F35" s="4" t="n"/>
+      <c r="A35" s="4" t="n"/>
+      <c r="B35" s="13" t="n"/>
+      <c r="C35" s="26" t="n"/>
+      <c r="D35" s="24" t="n"/>
+      <c r="E35" s="26" t="n"/>
+      <c r="F35" s="24" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="6" t="n"/>
-      <c r="B36" s="2" t="n"/>
-      <c r="C36" s="14" t="n"/>
-      <c r="D36" s="4" t="n"/>
-      <c r="E36" s="14" t="n"/>
-      <c r="F36" s="4" t="n"/>
+      <c r="A36" s="4" t="n"/>
+      <c r="B36" s="12" t="n"/>
+      <c r="C36" s="26" t="n"/>
+      <c r="D36" s="24" t="n"/>
+      <c r="E36" s="26" t="n"/>
+      <c r="F36" s="24" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="6" t="n"/>
-      <c r="B37" s="11" t="n"/>
-      <c r="C37" s="14" t="n"/>
-      <c r="D37" s="4" t="n"/>
-      <c r="E37" s="14" t="n"/>
-      <c r="F37" s="4" t="n"/>
+      <c r="A37" s="4" t="n"/>
+      <c r="B37" s="13" t="n"/>
+      <c r="C37" s="26" t="n"/>
+      <c r="D37" s="24" t="n"/>
+      <c r="E37" s="26" t="n"/>
+      <c r="F37" s="24" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="6" t="n"/>
-      <c r="B38" s="11" t="n"/>
-      <c r="C38" s="14" t="n"/>
-      <c r="D38" s="4" t="n"/>
-      <c r="E38" s="14" t="n"/>
-      <c r="F38" s="4" t="n"/>
+      <c r="A38" s="4" t="n"/>
+      <c r="B38" s="13" t="n"/>
+      <c r="C38" s="26" t="n"/>
+      <c r="D38" s="24" t="n"/>
+      <c r="E38" s="26" t="n"/>
+      <c r="F38" s="24" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="6" t="n"/>
-      <c r="B39" s="11" t="n"/>
-      <c r="C39" s="14" t="n"/>
-      <c r="D39" s="4" t="n"/>
-      <c r="E39" s="14" t="n"/>
-      <c r="F39" s="4" t="n"/>
+      <c r="A39" s="4" t="n"/>
+      <c r="B39" s="13" t="n"/>
+      <c r="C39" s="26" t="n"/>
+      <c r="D39" s="24" t="n"/>
+      <c r="E39" s="26" t="n"/>
+      <c r="F39" s="24" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="n"/>
-      <c r="B40" s="11" t="n"/>
-      <c r="C40" s="14" t="n"/>
-      <c r="D40" s="4" t="n"/>
-      <c r="E40" s="14" t="n"/>
-      <c r="F40" s="4" t="n"/>
+      <c r="A40" s="4" t="n"/>
+      <c r="B40" s="13" t="n"/>
+      <c r="C40" s="26" t="n"/>
+      <c r="D40" s="24" t="n"/>
+      <c r="E40" s="26" t="n"/>
+      <c r="F40" s="24" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="6" t="n"/>
-      <c r="B41" s="11" t="n"/>
-      <c r="C41" s="14" t="n"/>
-      <c r="D41" s="4" t="n"/>
-      <c r="E41" s="14" t="n"/>
-      <c r="F41" s="4" t="n"/>
+      <c r="A41" s="4" t="n"/>
+      <c r="B41" s="13" t="n"/>
+      <c r="C41" s="26" t="n"/>
+      <c r="D41" s="24" t="n"/>
+      <c r="E41" s="26" t="n"/>
+      <c r="F41" s="24" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="6" t="n"/>
-      <c r="B42" s="11" t="n"/>
-      <c r="C42" s="14" t="n"/>
-      <c r="D42" s="4" t="n"/>
-      <c r="E42" s="14" t="n"/>
-      <c r="F42" s="4" t="n"/>
+      <c r="A42" s="4" t="n"/>
+      <c r="B42" s="13" t="n"/>
+      <c r="C42" s="26" t="n"/>
+      <c r="D42" s="24" t="n"/>
+      <c r="E42" s="26" t="n"/>
+      <c r="F42" s="24" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="6" t="n"/>
-      <c r="B43" s="11" t="n"/>
-      <c r="C43" s="14" t="n"/>
-      <c r="D43" s="4" t="n"/>
-      <c r="E43" s="14" t="n"/>
-      <c r="F43" s="4" t="n"/>
+      <c r="A43" s="4" t="n"/>
+      <c r="B43" s="13" t="n"/>
+      <c r="C43" s="26" t="n"/>
+      <c r="D43" s="24" t="n"/>
+      <c r="E43" s="26" t="n"/>
+      <c r="F43" s="24" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="11" t="n"/>
-      <c r="C44" s="14" t="n"/>
-      <c r="D44" s="4" t="n"/>
-      <c r="E44" s="14" t="n"/>
-      <c r="F44" s="4" t="n"/>
+      <c r="A44" s="4" t="n"/>
+      <c r="B44" s="13" t="n"/>
+      <c r="C44" s="26" t="n"/>
+      <c r="D44" s="24" t="n"/>
+      <c r="E44" s="26" t="n"/>
+      <c r="F44" s="24" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
+      <c r="A45" s="4" t="n"/>
+      <c r="B45" s="21" t="n"/>
+      <c r="C45" s="27" t="n"/>
+      <c r="D45" s="27" t="n"/>
+      <c r="E45" s="27" t="n"/>
+      <c r="F45" s="27" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="13" t="n"/>
-      <c r="C46" s="14" t="n"/>
-      <c r="D46" s="14" t="n"/>
-      <c r="E46" s="14" t="n"/>
-      <c r="F46" s="14" t="n"/>
+      <c r="A46" s="4" t="n"/>
+      <c r="B46" s="11" t="n"/>
+      <c r="C46" s="26" t="n"/>
+      <c r="D46" s="26" t="n"/>
+      <c r="E46" s="26" t="n"/>
+      <c r="F46" s="26" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="6" t="n"/>
-      <c r="B47" s="18" t="n"/>
-      <c r="C47" s="14" t="n"/>
-      <c r="D47" s="4" t="n"/>
-      <c r="E47" s="14" t="n"/>
-      <c r="F47" s="4" t="n"/>
+      <c r="A47" s="4" t="n"/>
+      <c r="B47" s="13" t="n"/>
+      <c r="C47" s="26" t="n"/>
+      <c r="D47" s="24" t="n"/>
+      <c r="E47" s="26" t="n"/>
+      <c r="F47" s="24" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="6" t="n"/>
-      <c r="B48" s="18" t="n"/>
-      <c r="C48" s="14" t="n"/>
-      <c r="D48" s="4" t="n"/>
-      <c r="E48" s="14" t="n"/>
-      <c r="F48" s="4" t="n"/>
+      <c r="A48" s="4" t="n"/>
+      <c r="B48" s="13" t="n"/>
+      <c r="C48" s="26" t="n"/>
+      <c r="D48" s="24" t="n"/>
+      <c r="E48" s="26" t="n"/>
+      <c r="F48" s="24" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="6" t="n"/>
-      <c r="B49" s="11" t="n"/>
-      <c r="C49" s="14" t="n"/>
-      <c r="D49" s="4" t="n"/>
-      <c r="E49" s="14" t="n"/>
-      <c r="F49" s="4" t="n"/>
+      <c r="A49" s="4" t="n"/>
+      <c r="B49" s="13" t="n"/>
+      <c r="C49" s="26" t="n"/>
+      <c r="D49" s="24" t="n"/>
+      <c r="E49" s="26" t="n"/>
+      <c r="F49" s="24" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="n"/>
-      <c r="B50" s="11" t="n"/>
-      <c r="C50" s="14" t="n"/>
-      <c r="D50" s="4" t="n"/>
-      <c r="E50" s="14" t="n"/>
-      <c r="F50" s="4" t="n"/>
+      <c r="A50" s="4" t="n"/>
+      <c r="B50" s="13" t="n"/>
+      <c r="C50" s="26" t="n"/>
+      <c r="D50" s="24" t="n"/>
+      <c r="E50" s="26" t="n"/>
+      <c r="F50" s="24" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="6" t="n"/>
-      <c r="B51" s="11" t="n"/>
-      <c r="C51" s="14" t="n"/>
-      <c r="D51" s="4" t="n"/>
-      <c r="E51" s="14" t="n"/>
-      <c r="F51" s="4" t="n"/>
+      <c r="A51" s="4" t="n"/>
+      <c r="B51" s="13" t="n"/>
+      <c r="C51" s="26" t="n"/>
+      <c r="D51" s="24" t="n"/>
+      <c r="E51" s="26" t="n"/>
+      <c r="F51" s="24" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="6" t="n"/>
-      <c r="B52" s="2" t="n"/>
-      <c r="C52" s="14" t="n"/>
-      <c r="D52" s="4" t="n"/>
-      <c r="E52" s="14" t="n"/>
-      <c r="F52" s="4" t="n"/>
+      <c r="A52" s="4" t="n"/>
+      <c r="B52" s="12" t="n"/>
+      <c r="C52" s="26" t="n"/>
+      <c r="D52" s="24" t="n"/>
+      <c r="E52" s="26" t="n"/>
+      <c r="F52" s="24" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="6" t="n"/>
-      <c r="B53" s="11" t="n"/>
-      <c r="C53" s="14" t="n"/>
-      <c r="D53" s="4" t="n"/>
-      <c r="E53" s="14" t="n"/>
-      <c r="F53" s="4" t="n"/>
+      <c r="A53" s="4" t="n"/>
+      <c r="B53" s="13" t="n"/>
+      <c r="C53" s="26" t="n"/>
+      <c r="D53" s="24" t="n"/>
+      <c r="E53" s="26" t="n"/>
+      <c r="F53" s="24" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="n"/>
-      <c r="B54" s="11" t="n"/>
-      <c r="C54" s="14" t="n"/>
-      <c r="D54" s="4" t="n"/>
-      <c r="E54" s="14" t="n"/>
-      <c r="F54" s="4" t="n"/>
+      <c r="A54" s="4" t="n"/>
+      <c r="B54" s="13" t="n"/>
+      <c r="C54" s="26" t="n"/>
+      <c r="D54" s="24" t="n"/>
+      <c r="E54" s="26" t="n"/>
+      <c r="F54" s="24" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="6" t="n"/>
-      <c r="B55" s="11" t="n"/>
-      <c r="C55" s="14" t="n"/>
-      <c r="D55" s="4" t="n"/>
-      <c r="E55" s="14" t="n"/>
-      <c r="F55" s="4" t="n"/>
+      <c r="A55" s="4" t="n"/>
+      <c r="B55" s="13" t="n"/>
+      <c r="C55" s="26" t="n"/>
+      <c r="D55" s="24" t="n"/>
+      <c r="E55" s="26" t="n"/>
+      <c r="F55" s="24" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="6" t="n"/>
-      <c r="B56" s="11" t="n"/>
-      <c r="C56" s="14" t="n"/>
-      <c r="D56" s="4" t="n"/>
-      <c r="E56" s="14" t="n"/>
-      <c r="F56" s="4" t="n"/>
+      <c r="A56" s="4" t="n"/>
+      <c r="B56" s="13" t="n"/>
+      <c r="C56" s="26" t="n"/>
+      <c r="D56" s="24" t="n"/>
+      <c r="E56" s="26" t="n"/>
+      <c r="F56" s="24" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="6" t="n"/>
-      <c r="B57" s="11" t="n"/>
-      <c r="C57" s="14" t="n"/>
-      <c r="D57" s="4" t="n"/>
-      <c r="E57" s="14" t="n"/>
-      <c r="F57" s="4" t="n"/>
+      <c r="A57" s="4" t="n"/>
+      <c r="B57" s="13" t="n"/>
+      <c r="C57" s="26" t="n"/>
+      <c r="D57" s="24" t="n"/>
+      <c r="E57" s="26" t="n"/>
+      <c r="F57" s="24" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="6" t="n"/>
-      <c r="B58" s="11" t="n"/>
-      <c r="C58" s="14" t="n"/>
-      <c r="D58" s="4" t="n"/>
-      <c r="E58" s="14" t="n"/>
-      <c r="F58" s="4" t="n"/>
+      <c r="A58" s="4" t="n"/>
+      <c r="B58" s="13" t="n"/>
+      <c r="C58" s="26" t="n"/>
+      <c r="D58" s="24" t="n"/>
+      <c r="E58" s="26" t="n"/>
+      <c r="F58" s="24" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="6" t="n"/>
-      <c r="B59" s="11" t="n"/>
-      <c r="C59" s="14" t="n"/>
-      <c r="D59" s="4" t="n"/>
-      <c r="E59" s="14" t="n"/>
-      <c r="F59" s="4" t="n"/>
+      <c r="A59" s="4" t="n"/>
+      <c r="B59" s="13" t="n"/>
+      <c r="C59" s="26" t="n"/>
+      <c r="D59" s="24" t="n"/>
+      <c r="E59" s="26" t="n"/>
+      <c r="F59" s="24" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="6" t="n"/>
-      <c r="B60" s="11" t="n"/>
-      <c r="C60" s="14" t="n"/>
-      <c r="D60" s="4" t="n"/>
-      <c r="E60" s="14" t="n"/>
-      <c r="F60" s="4" t="n"/>
+      <c r="A60" s="4" t="n"/>
+      <c r="B60" s="13" t="n"/>
+      <c r="C60" s="26" t="n"/>
+      <c r="D60" s="24" t="n"/>
+      <c r="E60" s="26" t="n"/>
+      <c r="F60" s="24" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="6" t="n"/>
-      <c r="B61" s="6" t="n"/>
-      <c r="C61" s="6" t="n"/>
-      <c r="D61" s="6" t="n"/>
-      <c r="E61" s="6" t="n"/>
-      <c r="F61" s="6" t="n"/>
+      <c r="A61" s="4" t="n"/>
+      <c r="B61" s="21" t="n"/>
+      <c r="C61" s="27" t="n"/>
+      <c r="D61" s="27" t="n"/>
+      <c r="E61" s="27" t="n"/>
+      <c r="F61" s="27" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="6" t="n"/>
-      <c r="B62" s="13" t="n"/>
-      <c r="C62" s="14" t="n"/>
-      <c r="D62" s="14" t="n"/>
-      <c r="E62" s="14" t="n"/>
-      <c r="F62" s="14" t="n"/>
+      <c r="A62" s="4" t="n"/>
+      <c r="B62" s="11" t="n"/>
+      <c r="C62" s="26" t="n"/>
+      <c r="D62" s="26" t="n"/>
+      <c r="E62" s="26" t="n"/>
+      <c r="F62" s="26" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="6" t="n"/>
-      <c r="B63" s="18" t="n"/>
-      <c r="C63" s="14" t="n"/>
-      <c r="D63" s="4" t="n"/>
-      <c r="E63" s="14" t="n"/>
-      <c r="F63" s="4" t="n"/>
+      <c r="A63" s="4" t="n"/>
+      <c r="B63" s="13" t="n"/>
+      <c r="C63" s="26" t="n"/>
+      <c r="D63" s="24" t="n"/>
+      <c r="E63" s="26" t="n"/>
+      <c r="F63" s="24" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="6" t="n"/>
-      <c r="B64" s="18" t="n"/>
-      <c r="C64" s="14" t="n"/>
-      <c r="D64" s="4" t="n"/>
-      <c r="E64" s="14" t="n"/>
-      <c r="F64" s="4" t="n"/>
+      <c r="A64" s="4" t="n"/>
+      <c r="B64" s="13" t="n"/>
+      <c r="C64" s="26" t="n"/>
+      <c r="D64" s="24" t="n"/>
+      <c r="E64" s="26" t="n"/>
+      <c r="F64" s="24" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="6" t="n"/>
-      <c r="B65" s="11" t="n"/>
-      <c r="C65" s="14" t="n"/>
-      <c r="D65" s="4" t="n"/>
-      <c r="E65" s="14" t="n"/>
-      <c r="F65" s="4" t="n"/>
+      <c r="A65" s="4" t="n"/>
+      <c r="B65" s="13" t="n"/>
+      <c r="C65" s="26" t="n"/>
+      <c r="D65" s="24" t="n"/>
+      <c r="E65" s="26" t="n"/>
+      <c r="F65" s="24" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="6" t="n"/>
-      <c r="B66" s="11" t="n"/>
-      <c r="C66" s="14" t="n"/>
-      <c r="D66" s="4" t="n"/>
-      <c r="E66" s="14" t="n"/>
-      <c r="F66" s="4" t="n"/>
+      <c r="A66" s="4" t="n"/>
+      <c r="B66" s="13" t="n"/>
+      <c r="C66" s="26" t="n"/>
+      <c r="D66" s="24" t="n"/>
+      <c r="E66" s="26" t="n"/>
+      <c r="F66" s="24" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" s="6" t="n"/>
-      <c r="B67" s="11" t="n"/>
-      <c r="C67" s="14" t="n"/>
-      <c r="D67" s="4" t="n"/>
-      <c r="E67" s="14" t="n"/>
-      <c r="F67" s="4" t="n"/>
+      <c r="A67" s="4" t="n"/>
+      <c r="B67" s="13" t="n"/>
+      <c r="C67" s="26" t="n"/>
+      <c r="D67" s="24" t="n"/>
+      <c r="E67" s="26" t="n"/>
+      <c r="F67" s="24" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" s="6" t="n"/>
-      <c r="B68" s="2" t="n"/>
-      <c r="C68" s="14" t="n"/>
-      <c r="D68" s="4" t="n"/>
-      <c r="E68" s="14" t="n"/>
-      <c r="F68" s="4" t="n"/>
+      <c r="A68" s="4" t="n"/>
+      <c r="B68" s="12" t="n"/>
+      <c r="C68" s="26" t="n"/>
+      <c r="D68" s="24" t="n"/>
+      <c r="E68" s="26" t="n"/>
+      <c r="F68" s="24" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" s="6" t="n"/>
-      <c r="B69" s="11" t="n"/>
-      <c r="C69" s="14" t="n"/>
-      <c r="D69" s="4" t="n"/>
-      <c r="E69" s="14" t="n"/>
-      <c r="F69" s="4" t="n"/>
+      <c r="A69" s="4" t="n"/>
+      <c r="B69" s="13" t="n"/>
+      <c r="C69" s="26" t="n"/>
+      <c r="D69" s="24" t="n"/>
+      <c r="E69" s="26" t="n"/>
+      <c r="F69" s="24" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" s="6" t="n"/>
-      <c r="B70" s="11" t="n"/>
-      <c r="C70" s="14" t="n"/>
-      <c r="D70" s="4" t="n"/>
-      <c r="E70" s="14" t="n"/>
-      <c r="F70" s="4" t="n"/>
+      <c r="A70" s="4" t="n"/>
+      <c r="B70" s="13" t="n"/>
+      <c r="C70" s="26" t="n"/>
+      <c r="D70" s="24" t="n"/>
+      <c r="E70" s="26" t="n"/>
+      <c r="F70" s="24" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" s="6" t="n"/>
-      <c r="B71" s="11" t="n"/>
-      <c r="C71" s="14" t="n"/>
-      <c r="D71" s="4" t="n"/>
-      <c r="E71" s="15" t="n"/>
-      <c r="F71" s="4" t="n"/>
+      <c r="A71" s="4" t="n"/>
+      <c r="B71" s="13" t="n"/>
+      <c r="C71" s="26" t="n"/>
+      <c r="D71" s="24" t="n"/>
+      <c r="E71" s="25" t="n"/>
+      <c r="F71" s="24" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" s="6" t="n"/>
-      <c r="B72" s="11" t="n"/>
-      <c r="C72" s="14" t="n"/>
-      <c r="D72" s="4" t="n"/>
-      <c r="E72" s="14" t="n"/>
-      <c r="F72" s="4" t="n"/>
+      <c r="A72" s="4" t="n"/>
+      <c r="B72" s="13" t="n"/>
+      <c r="C72" s="26" t="n"/>
+      <c r="D72" s="24" t="n"/>
+      <c r="E72" s="26" t="n"/>
+      <c r="F72" s="24" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" s="6" t="n"/>
-      <c r="B73" s="11" t="n"/>
-      <c r="C73" s="14" t="n"/>
-      <c r="D73" s="4" t="n"/>
-      <c r="E73" s="14" t="n"/>
-      <c r="F73" s="4" t="n"/>
+      <c r="A73" s="4" t="n"/>
+      <c r="B73" s="13" t="n"/>
+      <c r="C73" s="26" t="n"/>
+      <c r="D73" s="24" t="n"/>
+      <c r="E73" s="26" t="n"/>
+      <c r="F73" s="24" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="6" t="n"/>
-      <c r="B74" s="11" t="n"/>
-      <c r="C74" s="14" t="n"/>
-      <c r="D74" s="4" t="n"/>
-      <c r="E74" s="14" t="n"/>
-      <c r="F74" s="4" t="n"/>
+      <c r="A74" s="4" t="n"/>
+      <c r="B74" s="13" t="n"/>
+      <c r="C74" s="26" t="n"/>
+      <c r="D74" s="24" t="n"/>
+      <c r="E74" s="26" t="n"/>
+      <c r="F74" s="24" t="n"/>
     </row>
     <row r="75">
-      <c r="A75" s="6" t="n"/>
-      <c r="B75" s="11" t="n"/>
-      <c r="C75" s="14" t="n"/>
-      <c r="D75" s="4" t="n"/>
-      <c r="E75" s="14" t="n"/>
-      <c r="F75" s="4" t="n"/>
+      <c r="A75" s="4" t="n"/>
+      <c r="B75" s="13" t="n"/>
+      <c r="C75" s="26" t="n"/>
+      <c r="D75" s="24" t="n"/>
+      <c r="E75" s="26" t="n"/>
+      <c r="F75" s="24" t="n"/>
     </row>
     <row r="76">
-      <c r="A76" s="6" t="n"/>
-      <c r="B76" s="11" t="n"/>
-      <c r="C76" s="14" t="n"/>
-      <c r="D76" s="4" t="n"/>
-      <c r="E76" s="14" t="n"/>
-      <c r="F76" s="4" t="n"/>
+      <c r="A76" s="4" t="n"/>
+      <c r="B76" s="13" t="n"/>
+      <c r="C76" s="26" t="n"/>
+      <c r="D76" s="24" t="n"/>
+      <c r="E76" s="26" t="n"/>
+      <c r="F76" s="24" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>